<commit_message>
exel sheet data test case
</commit_message>
<xml_diff>
--- a/DDT-Selenium/exelsheet/logindetails.xlsx
+++ b/DDT-Selenium/exelsheet/logindetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asad\Desktop\Selenium Projects\DDT-Selenium\exelsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAEFD32-4168-4A1B-A0C4-0953CED0218C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8440C2-F434-4AAC-B7F1-61AFFA4245DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Username</t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t>third</t>
+  </si>
+  <si>
+    <t>Sufiyan@gmail.com</t>
+  </si>
+  <si>
+    <t>fourth</t>
+  </si>
+  <si>
+    <t>Mumtaz@gmail.com</t>
+  </si>
+  <si>
+    <t>fifth</t>
   </si>
 </sst>
 </file>
@@ -377,9 +389,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -418,11 +432,29 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{DE7D170D-FDA2-4CEE-960B-0F3520536B2B}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{2BF7AB5C-B86C-42FA-8B22-0211B7331670}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{8B6FB62B-F4DA-4836-B50A-6C6A61FCB400}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{BE91D707-D84F-45BF-B653-B420BFDFEF19}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{7F7FCA57-D650-4423-BFE6-A0B66FC74BEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>